<commit_message>
edits to FCproc for Quest
</commit_message>
<xml_diff>
--- a/FCProcess/EXAMPLESUB_DATALIST.xlsx
+++ b/FCProcess/EXAMPLESUB_DATALIST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgv5452/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgratton/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23B61FAF-CC27-414E-B589-BACCFB988900}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD391867-593A-4F43-8241-0F6F59EC755B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17520" yWindow="1040" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="17520" yWindow="1040" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EXAMPLESUB_DATALIST" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>/projects/b1081/iNetworks/Nifti/derivatives</t>
   </si>
   <si>
-    <t>preproc_fmriprep-1.5.8_MOD5</t>
-  </si>
-  <si>
     <t>1,2,3,4,5,6,7</t>
   </si>
   <si>
@@ -74,12 +71,15 @@
   </si>
   <si>
     <t>1,2,3,4,5,6,7,8</t>
+  </si>
+  <si>
+    <t>preproc_fmriprep-20.0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -913,11 +913,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,16 +974,16 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1006,16 +1006,16 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1038,16 +1038,16 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
         <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1070,16 +1070,16 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to mask and nuis regression
</commit_message>
<xml_diff>
--- a/FCProcess/EXAMPLESUB_DATALIST.xlsx
+++ b/FCProcess/EXAMPLESUB_DATALIST.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgratton/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgv5452/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD391867-593A-4F43-8241-0F6F59EC755B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A618E763-2F7F-0444-A0C0-182B5499F628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17520" yWindow="1040" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
     <t>1,2,3,4,5,6,7,8</t>
   </si>
   <si>
-    <t>preproc_fmriprep-20.0.1</t>
+    <t>preproc_fmriprep-20.0.6</t>
   </si>
 </sst>
 </file>
@@ -917,7 +917,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>